<commit_message>
added Rosenbauer ME cover letter
</commit_message>
<xml_diff>
--- a/job_list.xlsx
+++ b/job_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakob\projects\portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E6B6AA-F4CC-4F65-B61A-91DFECB8F7EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E830090-00BB-4E37-8B7B-851A406823CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{BA7AE640-4DA0-4C72-86A8-5C328AB94AC8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="63">
   <si>
     <t>Company</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>Job post disappeared after a few days…</t>
+  </si>
+  <si>
+    <t>Test Cell Technician</t>
   </si>
 </sst>
 </file>
@@ -575,8 +578,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{22F06905-C2D9-48C2-A7CA-A0EB530B5540}" name="Table1" displayName="Table1" ref="A1:I19" totalsRowShown="0" headerRowDxfId="30">
-  <autoFilter ref="A1:I19" xr:uid="{22F06905-C2D9-48C2-A7CA-A0EB530B5540}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{22F06905-C2D9-48C2-A7CA-A0EB530B5540}" name="Table1" displayName="Table1" ref="A1:I20" totalsRowShown="0" headerRowDxfId="30">
+  <autoFilter ref="A1:I20" xr:uid="{22F06905-C2D9-48C2-A7CA-A0EB530B5540}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{373BECF1-87DB-4E32-A050-6B1C58A2CEFE}" name="Company"/>
     <tableColumn id="2" xr3:uid="{19167977-DEB2-4046-A945-56D2433D5E98}" name="Role"/>
@@ -909,10 +912,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13A8EF18-83C9-43D4-850E-545EF3A56400}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1145,9 +1148,11 @@
         <v>17</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="2"/>
+        <v>52</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="H9" s="2"/>
       <c r="I9" t="s">
         <v>19</v>
@@ -1207,7 +1212,9 @@
         <v>24</v>
       </c>
       <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="H12" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="I12" t="s">
         <v>61</v>
       </c>
@@ -1334,31 +1341,53 @@
       <c r="F19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="I19" t="s">
         <v>59</v>
       </c>
     </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:E19">
+  <conditionalFormatting sqref="D2:E20">
     <cfRule type="containsText" dxfId="23" priority="17" operator="containsText" text="In progress">
       <formula>NOT(ISERROR(SEARCH("In progress",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:F19">
+  <conditionalFormatting sqref="D2:F20">
     <cfRule type="containsBlanks" dxfId="22" priority="18">
       <formula>LEN(TRIM(D2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:G19">
+  <conditionalFormatting sqref="D2:G20">
     <cfRule type="containsText" dxfId="21" priority="16" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F19">
+  <conditionalFormatting sqref="F2:F20">
     <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="Called">
       <formula>NOT(ISERROR(SEARCH("Called",F2)))</formula>
     </cfRule>
@@ -1375,12 +1404,12 @@
       <formula>NOT(ISERROR(SEARCH("Need contact",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G19">
+  <conditionalFormatting sqref="G2:G20">
     <cfRule type="containsText" dxfId="15" priority="7" operator="containsText" text="Planning">
       <formula>NOT(ISERROR(SEARCH("Planning",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H19">
+  <conditionalFormatting sqref="H2:H20">
     <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Declined">
       <formula>NOT(ISERROR(SEARCH("Declined",H2)))</formula>
     </cfRule>
@@ -1392,16 +1421,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E19" xr:uid="{1C9B2CB6-A7FA-4A47-AF1B-899E854E8040}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E20" xr:uid="{1C9B2CB6-A7FA-4A47-AF1B-899E854E8040}">
       <formula1>"In progress,Done"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H19" xr:uid="{FCD6A7C9-AC00-44BE-B019-6C6D843484E8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H20" xr:uid="{FCD6A7C9-AC00-44BE-B019-6C6D843484E8}">
       <formula1>"Waiting, Received, Declined"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F19" xr:uid="{77321022-E098-4A3F-95A5-239C6D5C52BB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F20" xr:uid="{77321022-E098-4A3F-95A5-239C6D5C52BB}">
       <formula1>"Got response, LinkedIn, Emailed, Called"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G19" xr:uid="{A07026C2-D8B6-4A3E-B583-95F0161D8711}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G20" xr:uid="{A07026C2-D8B6-4A3E-B583-95F0161D8711}">
       <formula1>"Planning, Done"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
made bobcat cover letter, updated job list
</commit_message>
<xml_diff>
--- a/job_list.xlsx
+++ b/job_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakob\projects\portfolio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakob/projects/portfolio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E830090-00BB-4E37-8B7B-851A406823CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67B97E0-FCBE-C947-8561-5913CF0471FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{BA7AE640-4DA0-4C72-86A8-5C328AB94AC8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{BA7AE640-4DA0-4C72-86A8-5C328AB94AC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="78">
   <si>
     <t>Company</t>
   </si>
@@ -170,9 +170,6 @@
     <t>Robust info pages could help tailer my info</t>
   </si>
   <si>
-    <t>https://www.jobs.abbott/us/en/job/ABLAUS31109016ENUSEXTERNAL/Manufacturing-Engineer-I</t>
-  </si>
-  <si>
     <t>https://www.jobs.abbott/us/en/job/31101652/Process-Development-Engineer-I</t>
   </si>
   <si>
@@ -215,9 +212,6 @@
     <t>https://bostonscientific.eightfold.ai/careers/job/563602799718050?domain=bostonscientific.com&amp;hl=en</t>
   </si>
   <si>
-    <t>No option for CL. LinkedIn --&gt; Josh Kuechenmeister (mfg eng sprvsr)</t>
-  </si>
-  <si>
     <t>Planning</t>
   </si>
   <si>
@@ -225,6 +219,57 @@
   </si>
   <si>
     <t>Test Cell Technician</t>
+  </si>
+  <si>
+    <t>Doosan Bobcat</t>
+  </si>
+  <si>
+    <t>Manfucaturing Engineer</t>
+  </si>
+  <si>
+    <t>https://jobs.doosan.com/job/Rogers-Manufacturing-Engineer-MN-55374/1260590300/</t>
+  </si>
+  <si>
+    <t>LinkedIn --&gt; Josh Kuechenmeister (mfg eng sprvsr) career goals interview. No option for CL.</t>
+  </si>
+  <si>
+    <t>Response</t>
+  </si>
+  <si>
+    <t>Stopped replying</t>
+  </si>
+  <si>
+    <t>No response</t>
+  </si>
+  <si>
+    <t>Lucid Labs</t>
+  </si>
+  <si>
+    <t>Recruiter</t>
+  </si>
+  <si>
+    <t>Dude on linkedin --&gt; recruiter Matthew Rosson</t>
+  </si>
+  <si>
+    <t>linkedin</t>
+  </si>
+  <si>
+    <t>HR said that my info would be kept in system from last interview</t>
+  </si>
+  <si>
+    <t>Systems Engineer</t>
+  </si>
+  <si>
+    <t>https://www.polaris.com/en-us/careers/job-categories/engineering/apply/r25137/</t>
+  </si>
+  <si>
+    <t>https://www.paycomonline.net/v4/ats/web.php/jobs/ViewJobDetails?job=260359&amp;clientkey=03F49D0846EF4AAF221BF3C05F433A0E&amp;src=LinkedIn</t>
+  </si>
+  <si>
+    <t>R&amp;D Project Engineer - Mechanical</t>
+  </si>
+  <si>
+    <t>https://www.jobs.abbott/us/en/job/ABLAUS31109593ENUSEXTERNAL/Manufacturing-Engineer-I?utm_source=linkedin&amp;utm_medium=phenom-feeds</t>
   </si>
 </sst>
 </file>
@@ -248,12 +293,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -268,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -282,11 +333,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="44">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -329,6 +387,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -339,6 +417,46 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -369,6 +487,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -389,6 +517,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -399,6 +537,46 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -449,6 +627,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -459,6 +657,46 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -468,64 +706,7 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -578,17 +759,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{22F06905-C2D9-48C2-A7CA-A0EB530B5540}" name="Table1" displayName="Table1" ref="A1:I20" totalsRowShown="0" headerRowDxfId="30">
-  <autoFilter ref="A1:I20" xr:uid="{22F06905-C2D9-48C2-A7CA-A0EB530B5540}"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{22F06905-C2D9-48C2-A7CA-A0EB530B5540}" name="Table1" displayName="Table1" ref="A1:J25" totalsRowShown="0" headerRowDxfId="43">
+  <autoFilter ref="A1:J25" xr:uid="{22F06905-C2D9-48C2-A7CA-A0EB530B5540}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J23">
+    <sortCondition ref="I1:I23"/>
+  </sortState>
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{373BECF1-87DB-4E32-A050-6B1C58A2CEFE}" name="Company"/>
     <tableColumn id="2" xr3:uid="{19167977-DEB2-4046-A945-56D2433D5E98}" name="Role"/>
-    <tableColumn id="3" xr3:uid="{E4DE4438-9C7B-4D44-AC54-CA0FE413F8D6}" name="Source" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{CD12B571-B108-4E55-A7EA-B89A813BA2D0}" name="CL" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{3FD6CB17-5BEB-45C4-98BC-D5DD2E302C95}" name="Applied" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{A9A47AF1-716B-44C7-BD65-33E400C4C955}" name="Contacted" dataDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{F8254EA3-5FCC-4F56-9506-E5D3090C41E1}" name="Interview" dataDxfId="25"/>
-    <tableColumn id="8" xr3:uid="{961BE192-D722-4D7E-B60D-BF416EDA25D6}" name="Job Offer" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{E4DE4438-9C7B-4D44-AC54-CA0FE413F8D6}" name="Source" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{CD12B571-B108-4E55-A7EA-B89A813BA2D0}" name="CL" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{3FD6CB17-5BEB-45C4-98BC-D5DD2E302C95}" name="Applied" dataDxfId="40"/>
+    <tableColumn id="6" xr3:uid="{A9A47AF1-716B-44C7-BD65-33E400C4C955}" name="Contacted" dataDxfId="39"/>
+    <tableColumn id="10" xr3:uid="{E9EA5858-E491-8248-98A3-3B9E139C9FC8}" name="Response" dataDxfId="38"/>
+    <tableColumn id="7" xr3:uid="{F8254EA3-5FCC-4F56-9506-E5D3090C41E1}" name="Interview" dataDxfId="37"/>
+    <tableColumn id="8" xr3:uid="{961BE192-D722-4D7E-B60D-BF416EDA25D6}" name="Job Offer" dataDxfId="36"/>
     <tableColumn id="9" xr3:uid="{75E65A10-9DF4-46F8-BEA5-5708A22371C7}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -912,25 +1097,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13A8EF18-83C9-43D4-850E-545EF3A56400}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.05078125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.3125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5234375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5234375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.20703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.68359375" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -947,19 +1133,22 @@
         <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>38</v>
       </c>
@@ -972,24 +1161,27 @@
         <v>17</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>21</v>
+    <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="2" t="s">
@@ -1001,18 +1193,25 @@
       <c r="F3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>31</v>
+      <c r="G3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="2" t="s">
@@ -1024,18 +1223,25 @@
       <c r="F4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="G4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="2" t="s">
@@ -1045,24 +1251,27 @@
         <v>17</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="H5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="2" t="s">
@@ -1072,24 +1281,22 @@
         <v>17</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
-        <v>50</v>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="2" t="s">
@@ -1099,19 +1306,25 @@
         <v>17</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
+      <c r="J7" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="2" t="s">
@@ -1121,24 +1334,25 @@
         <v>17</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J8" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="2" t="s">
@@ -1148,290 +1362,437 @@
         <v>17</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="H9" s="2"/>
-      <c r="I9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="I9" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="H10" s="2"/>
-      <c r="I10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="I10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="H11" s="2"/>
-      <c r="I11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="I11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="F12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="H12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+        <v>17</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+        <v>55</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="E14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="B15" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="H15" s="2"/>
-      <c r="I15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="I15" s="2"/>
+      <c r="J15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+        <v>63</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="H16" s="2"/>
-      <c r="I16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="I16" s="2"/>
+      <c r="J16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
-      <c r="I17" t="s">
+      <c r="I17" s="2"/>
+      <c r="J17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D19" s="2"/>
-      <c r="E19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-      <c r="H19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="B24" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+    </row>
+    <row r="25" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:E20">
-    <cfRule type="containsText" dxfId="23" priority="17" operator="containsText" text="In progress">
+  <conditionalFormatting sqref="D2:E25">
+    <cfRule type="containsText" dxfId="35" priority="21" operator="containsText" text="In progress">
       <formula>NOT(ISERROR(SEARCH("In progress",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:F20">
-    <cfRule type="containsBlanks" dxfId="22" priority="18">
+  <conditionalFormatting sqref="D2:F25">
+    <cfRule type="containsBlanks" dxfId="34" priority="22">
       <formula>LEN(TRIM(D2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:G20">
-    <cfRule type="containsText" dxfId="21" priority="16" operator="containsText" text="Done">
+  <conditionalFormatting sqref="D2:H25">
+    <cfRule type="containsText" dxfId="33" priority="20" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F20">
-    <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="Called">
-      <formula>NOT(ISERROR(SEARCH("Called",F2)))</formula>
+  <conditionalFormatting sqref="F2:F25">
+    <cfRule type="notContainsBlanks" dxfId="32" priority="1">
+      <formula>LEN(TRIM(F2))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="2" operator="containsText" text="Emailed">
-      <formula>NOT(ISERROR(SEARCH("Emailed",F2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="3" operator="containsText" text="Got response">
-      <formula>NOT(ISERROR(SEARCH("Got response",F2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="4" operator="containsText" text="LInkedIn">
-      <formula>NOT(ISERROR(SEARCH("LInkedIn",F2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="9" operator="containsText" text="Need contact">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:G25">
+    <cfRule type="containsText" dxfId="31" priority="13" stopIfTrue="1" operator="containsText" text="Need contact">
       <formula>NOT(ISERROR(SEARCH("Need contact",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G20">
-    <cfRule type="containsText" dxfId="15" priority="7" operator="containsText" text="Planning">
-      <formula>NOT(ISERROR(SEARCH("Planning",G2)))</formula>
+  <conditionalFormatting sqref="G2:G25">
+    <cfRule type="containsText" dxfId="30" priority="2" stopIfTrue="1" operator="containsText" text="No response">
+      <formula>NOT(ISERROR(SEARCH("No response",G2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="29" priority="3" operator="containsText" text="Stopped replying">
+      <formula>NOT(ISERROR(SEARCH("Stopped replying",G2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="4" operator="containsText" text="Got response">
+      <formula>NOT(ISERROR(SEARCH("Got response",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H20">
-    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Declined">
-      <formula>NOT(ISERROR(SEARCH("Declined",H2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Waiting">
-      <formula>NOT(ISERROR(SEARCH("Waiting",H2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Recieved">
-      <formula>NOT(ISERROR(SEARCH("Recieved",H2)))</formula>
+  <conditionalFormatting sqref="H2:H25">
+    <cfRule type="containsText" dxfId="27" priority="11" operator="containsText" text="Planning">
+      <formula>NOT(ISERROR(SEARCH("Planning",H2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E20" xr:uid="{1C9B2CB6-A7FA-4A47-AF1B-899E854E8040}">
+  <conditionalFormatting sqref="I2:I25">
+    <cfRule type="containsText" dxfId="26" priority="17" operator="containsText" text="Declined">
+      <formula>NOT(ISERROR(SEARCH("Declined",I2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="18" operator="containsText" text="Waiting">
+      <formula>NOT(ISERROR(SEARCH("Waiting",I2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="19" operator="containsText" text="Recieved">
+      <formula>NOT(ISERROR(SEARCH("Recieved",I2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:E25" xr:uid="{1C9B2CB6-A7FA-4A47-AF1B-899E854E8040}">
       <formula1>"In progress,Done"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H20" xr:uid="{FCD6A7C9-AC00-44BE-B019-6C6D843484E8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I25" xr:uid="{FCD6A7C9-AC00-44BE-B019-6C6D843484E8}">
       <formula1>"Waiting, Received, Declined"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F20" xr:uid="{77321022-E098-4A3F-95A5-239C6D5C52BB}">
-      <formula1>"Got response, LinkedIn, Emailed, Called"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F25" xr:uid="{77321022-E098-4A3F-95A5-239C6D5C52BB}">
+      <formula1>"LinkedIn, Emailed, Called, Recruiter"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G20" xr:uid="{A07026C2-D8B6-4A3E-B583-95F0161D8711}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H25" xr:uid="{A07026C2-D8B6-4A3E-B583-95F0161D8711}">
       <formula1>"Planning, Done"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G25" xr:uid="{499D4362-04CD-534F-8FA1-EB7D325155C2}">
+      <formula1>"No response, Stopped replying, Got response"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>